<commit_message>
Added summary of metrics
</commit_message>
<xml_diff>
--- a/metrics_causal_mult_runs.xlsx
+++ b/metrics_causal_mult_runs.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amogh/Academic/Cambridge/L65/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909A2034-5194-D746-AA57-311D82A9C03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F11475-1F20-204D-999B-B392F61C4712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{CAC718FA-1DA9-5F4A-B975-0FDA83AFA7A5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{CAC718FA-1DA9-5F4A-B975-0FDA83AFA7A5}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="8" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId2"/>
-    <pivotCache cacheId="11" r:id="rId3"/>
-    <pivotCache cacheId="17" r:id="rId4"/>
-    <pivotCache cacheId="23" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="3" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="82">
   <si>
     <t>Metric</t>
   </si>
@@ -118,12 +119,183 @@
   <si>
     <t>Var</t>
   </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Dataset / Split</t>
+  </si>
+  <si>
+    <t>1 ± 2.9</t>
+  </si>
+  <si>
+    <t>4 ± 2.52</t>
+  </si>
+  <si>
+    <t>4.4 ± 2.9</t>
+  </si>
+  <si>
+    <t>4.6 ± 0.49</t>
+  </si>
+  <si>
+    <t>4.2 ± 0.4</t>
+  </si>
+  <si>
+    <t>4 ± 0</t>
+  </si>
+  <si>
+    <t>19.4 ± 2.57</t>
+  </si>
+  <si>
+    <t>17 ± 0.89</t>
+  </si>
+  <si>
+    <t>18.4 ± 2.72</t>
+  </si>
+  <si>
+    <t>44 ± 3.22</t>
+  </si>
+  <si>
+    <t>44.2 ± 4.7</t>
+  </si>
+  <si>
+    <t>44.8 ± 3.66</t>
+  </si>
+  <si>
+    <t>PC - Algorithm - SHD - Mean ± StdDev</t>
+  </si>
+  <si>
+    <t>Lingam - Corr - Mean ± StdDev</t>
+  </si>
+  <si>
+    <t>GES - SHD - Mean ± StdDev</t>
+  </si>
+  <si>
+    <t>3 ± 0</t>
+  </si>
+  <si>
+    <t>4.8 ± 1.93</t>
+  </si>
+  <si>
+    <t>4.4 ± 1.96</t>
+  </si>
+  <si>
+    <t>3.2 ± 0.75</t>
+  </si>
+  <si>
+    <t>3.6 ± 0.49</t>
+  </si>
+  <si>
+    <t>4 ± 1.55</t>
+  </si>
+  <si>
+    <t>32 ± 3.52</t>
+  </si>
+  <si>
+    <t>32.8 ± 0.98</t>
+  </si>
+  <si>
+    <t>29.2 ± 3.54</t>
+  </si>
+  <si>
+    <t>49.2 ± 10.49</t>
+  </si>
+  <si>
+    <t>36.8 ± 19.95</t>
+  </si>
+  <si>
+    <t>44.2 ± 9.32</t>
+  </si>
+  <si>
+    <t>FullCorr</t>
+  </si>
+  <si>
+    <t>SplitCorr</t>
+  </si>
+  <si>
+    <t>0.72 ± 0.15</t>
+  </si>
+  <si>
+    <t>0.54 ± 0.26</t>
+  </si>
+  <si>
+    <t>0.73 ± 0.1</t>
+  </si>
+  <si>
+    <t>0.74 ± 0.14</t>
+  </si>
+  <si>
+    <t>0.50 ± 0.24</t>
+  </si>
+  <si>
+    <t>0.67 ± 0.18</t>
+  </si>
+  <si>
+    <t>0.88 ± 0.11</t>
+  </si>
+  <si>
+    <t>0.79 ± 0.09</t>
+  </si>
+  <si>
+    <t>0.93 ± 0.03</t>
+  </si>
+  <si>
+    <t>0.96 ± 0.04</t>
+  </si>
+  <si>
+    <t>0.82 ± 0.12</t>
+  </si>
+  <si>
+    <t>0.76 ± 0.09</t>
+  </si>
+  <si>
+    <t>0.20 ± 0.06</t>
+  </si>
+  <si>
+    <t>0.23 ± 0.13</t>
+  </si>
+  <si>
+    <t>0.29 ± 0.18</t>
+  </si>
+  <si>
+    <t>0.18 ± 0.05</t>
+  </si>
+  <si>
+    <t>0.19 ± 0.08</t>
+  </si>
+  <si>
+    <t>0.2 ± 0.15</t>
+  </si>
+  <si>
+    <t>0.28 ± 0.06</t>
+  </si>
+  <si>
+    <t>0.37 ± 0.1</t>
+  </si>
+  <si>
+    <t>0.30 ± 0.11</t>
+  </si>
+  <si>
+    <t>0.25 ± 0.03</t>
+  </si>
+  <si>
+    <t>0.33 ± 0.08</t>
+  </si>
+  <si>
+    <t>0.24 ± 0.11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,16 +309,57 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -154,16 +367,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -174,7 +444,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2082,7 +2376,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A37CCFF-06E5-964E-A29F-EB584EBDD27A}" name="PivotTable4" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A37CCFF-06E5-964E-A29F-EB584EBDD27A}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G34:J58" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -2222,7 +2516,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9B6B01D-477A-1E4F-A19B-C3B490BB6DE5}" name="PivotTable3" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E9B6B01D-477A-1E4F-A19B-C3B490BB6DE5}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="Q6:T30" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -2362,7 +2656,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7ED994AA-AC60-4A48-9A61-B887005D2EAA}" name="PivotTable2" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7ED994AA-AC60-4A48-9A61-B887005D2EAA}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L6:O30" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -2502,7 +2796,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{90CA7EE1-07F7-CD43-AF04-F9ED4708F441}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{90CA7EE1-07F7-CD43-AF04-F9ED4708F441}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G6:J30" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -2703,6 +2997,32 @@
     <tableColumn id="3" xr3:uid="{737009C3-A059-FA4B-90C1-328701990BAC}" name="Split"/>
     <tableColumn id="4" xr3:uid="{C4D7F231-E4A9-104F-BDCD-76D85A44BE6E}" name="Metric"/>
     <tableColumn id="5" xr3:uid="{66EC2639-D72B-B247-81E7-AD89E015F834}" name="Value" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2CFE68E-FF32-944F-8CCC-C1FEFDEAECEF}" name="Table1" displayName="Table1" ref="B3:E7" totalsRowShown="0">
+  <autoFilter ref="B3:E7" xr:uid="{F2CFE68E-FF32-944F-8CCC-C1FEFDEAECEF}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{EC3D1D8E-F71C-DE4B-9A4D-8ECC13DADE53}" name="Dataset / Split"/>
+    <tableColumn id="2" xr3:uid="{4A01F70F-85A5-6E42-B096-5E944FD5469D}" name="Train"/>
+    <tableColumn id="3" xr3:uid="{393B5114-8FA5-EC40-91D6-746FE528D157}" name="Val"/>
+    <tableColumn id="4" xr3:uid="{EA643041-7C94-F94C-BF2D-90FCC0A2D754}" name="Test"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{32EC6F40-95E6-E64A-A243-85119197BAE5}" name="Table2" displayName="Table2" ref="B11:E15" totalsRowShown="0">
+  <autoFilter ref="B11:E15" xr:uid="{32EC6F40-95E6-E64A-A243-85119197BAE5}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8208B7CA-3AC7-9343-ACE6-67C57A92485A}" name="Dataset / Split"/>
+    <tableColumn id="2" xr3:uid="{6EA07B14-FAB5-334D-83AE-4095A17E2D77}" name="Train"/>
+    <tableColumn id="3" xr3:uid="{A8CF1846-E518-A44C-86A8-9BDB87D668CC}" name="Val"/>
+    <tableColumn id="4" xr3:uid="{F85A2891-90FF-D442-A15A-33771CC44728}" name="Test"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3027,8 +3347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B57365-7067-3945-B2A4-94FFD8293DDC}">
   <dimension ref="A1:T271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43:J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3214,21 +3534,12 @@
       <c r="G7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
       <c r="L7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
       <c r="Q7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -3249,21 +3560,12 @@
       <c r="G8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
       <c r="L8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
       <c r="Q8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -3284,37 +3586,37 @@
       <c r="G9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9">
         <v>1.9595917942265424</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9">
         <v>3.84</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M9" s="9">
-        <v>4</v>
-      </c>
-      <c r="N9" s="9">
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
         <v>1.5491933384829668</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9">
         <v>2.4</v>
       </c>
       <c r="Q9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R9" s="9">
+      <c r="R9">
         <v>29.2</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9">
         <v>3.54400902933387</v>
       </c>
-      <c r="T9" s="9">
+      <c r="T9">
         <v>12.56</v>
       </c>
     </row>
@@ -3337,21 +3639,12 @@
       <c r="G10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
       <c r="L10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
       <c r="Q10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -3372,37 +3665,37 @@
       <c r="G11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="9">
-        <v>3</v>
-      </c>
-      <c r="I11" s="9">
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
         <v>0</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11">
         <v>0</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11">
         <v>3.2</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11">
         <v>0.74833147735478833</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11">
         <v>0.56000000000000005</v>
       </c>
       <c r="Q11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R11" s="9">
+      <c r="R11">
         <v>32</v>
       </c>
-      <c r="S11" s="9">
+      <c r="S11">
         <v>3.5213633723318019</v>
       </c>
-      <c r="T11" s="9">
+      <c r="T11">
         <v>12.4</v>
       </c>
     </row>
@@ -3425,21 +3718,12 @@
       <c r="G12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
       <c r="L12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
       <c r="Q12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -3460,37 +3744,37 @@
       <c r="G13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13">
         <v>4.8</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13">
         <v>1.9390719429665315</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13">
         <v>3.76</v>
       </c>
       <c r="L13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13">
         <v>3.6</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13">
         <v>0.4898979485566356</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13">
         <v>0.24</v>
       </c>
       <c r="Q13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R13" s="9">
+      <c r="R13">
         <v>32.799999999999997</v>
       </c>
-      <c r="S13" s="9">
+      <c r="S13">
         <v>0.9797958971132712</v>
       </c>
-      <c r="T13" s="9">
+      <c r="T13">
         <v>0.96</v>
       </c>
     </row>
@@ -3513,21 +3797,12 @@
       <c r="G14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
       <c r="L14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
       <c r="Q14" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -3548,21 +3823,12 @@
       <c r="G15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
       <c r="L15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
       <c r="Q15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -3583,37 +3849,37 @@
       <c r="G16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16">
         <v>0.67207430340557228</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16">
         <v>0.17791750290249148</v>
       </c>
-      <c r="J16" s="9">
+      <c r="J16">
         <v>3.1654637839058065E-2</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16">
         <v>0.76354978354978331</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16">
         <v>9.2760532593953018E-2</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16">
         <v>8.6045164071138196E-3</v>
       </c>
       <c r="Q16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="R16" s="9">
+      <c r="R16">
         <v>0.19992342302835478</v>
       </c>
-      <c r="S16" s="9">
+      <c r="S16">
         <v>0.15098234208735042</v>
       </c>
-      <c r="T16" s="9">
+      <c r="T16">
         <v>2.2795667622181708E-2</v>
       </c>
     </row>
@@ -3636,37 +3902,37 @@
       <c r="G17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17">
         <v>0.73464646464646444</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17">
         <v>9.6365753952549454E-2</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17">
         <v>9.2863585348433014E-3</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="9">
+      <c r="M17">
         <v>0.9558974358974357</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17">
         <v>3.6203820707126085E-2</v>
       </c>
-      <c r="O17" s="9">
+      <c r="O17">
         <v>1.3107166337937314E-3</v>
       </c>
       <c r="Q17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="R17" s="9">
+      <c r="R17">
         <v>0.29560067386285621</v>
       </c>
-      <c r="S17" s="9">
+      <c r="S17">
         <v>0.17946848966341988</v>
       </c>
-      <c r="T17" s="9">
+      <c r="T17">
         <v>3.2208938782069048E-2</v>
       </c>
     </row>
@@ -3689,21 +3955,12 @@
       <c r="G18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
       <c r="L18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
       <c r="Q18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -3724,37 +3981,37 @@
       <c r="G19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19">
         <v>0.73781557967316425</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19">
         <v>0.14071207192700261</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19">
         <v>1.9799887185989958E-2</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19">
         <v>0.82060606060606034</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19">
         <v>0.12070195669822682</v>
       </c>
-      <c r="O19" s="9">
+      <c r="O19">
         <v>1.4568962350780623E-2</v>
       </c>
       <c r="Q19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="R19" s="9">
+      <c r="R19">
         <v>0.18003996599329192</v>
       </c>
-      <c r="S19" s="9">
+      <c r="S19">
         <v>5.0212363492822029E-2</v>
       </c>
-      <c r="T19" s="9">
+      <c r="T19">
         <v>2.5212814475352864E-3</v>
       </c>
     </row>
@@ -3777,37 +4034,37 @@
       <c r="G20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20">
         <v>0.71835667600373421</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20">
         <v>0.14637604274722904</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20">
         <v>2.1425945890338624E-2</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20">
         <v>0.88158508158508142</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20">
         <v>0.11264699905297117</v>
       </c>
-      <c r="O20" s="9">
+      <c r="O20">
         <v>1.2689346395640087E-2</v>
       </c>
       <c r="Q20" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="R20" s="9">
+      <c r="R20">
         <v>0.20493444456173462</v>
       </c>
-      <c r="S20" s="9">
+      <c r="S20">
         <v>5.7741306378144834E-2</v>
       </c>
-      <c r="T20" s="9">
+      <c r="T20">
         <v>3.3340584622547896E-3</v>
       </c>
     </row>
@@ -3830,21 +4087,12 @@
       <c r="G21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
       <c r="L21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
       <c r="Q21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -3865,37 +4113,37 @@
       <c r="G22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22">
         <v>0.49809523809523759</v>
       </c>
-      <c r="I22" s="9">
+      <c r="I22">
         <v>0.23659719206388971</v>
       </c>
-      <c r="J22" s="9">
+      <c r="J22">
         <v>5.5978231292517118E-2</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="9">
+      <c r="M22">
         <v>0.79006993006992976</v>
       </c>
-      <c r="N22" s="9">
+      <c r="N22">
         <v>8.8128363921315123E-2</v>
       </c>
-      <c r="O22" s="9">
+      <c r="O22">
         <v>7.7666085274477577E-3</v>
       </c>
       <c r="Q22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="R22" s="9">
+      <c r="R22">
         <v>0.18970564215683039</v>
       </c>
-      <c r="S22" s="9">
+      <c r="S22">
         <v>7.6080008837365071E-2</v>
       </c>
-      <c r="T22" s="9">
+      <c r="T22">
         <v>5.7881677446935467E-3</v>
       </c>
     </row>
@@ -3918,37 +4166,37 @@
       <c r="G23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23">
         <v>0.53976705306628525</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23">
         <v>0.262193185230229</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23">
         <v>6.8745266381173162E-2</v>
       </c>
       <c r="L23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M23" s="9">
+      <c r="M23">
         <v>0.93566433566433571</v>
       </c>
-      <c r="N23" s="9">
+      <c r="N23">
         <v>3.2620709901229686E-2</v>
       </c>
-      <c r="O23" s="9">
+      <c r="O23">
         <v>1.0641107144601846E-3</v>
       </c>
       <c r="Q23" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="R23" s="9">
+      <c r="R23">
         <v>0.22578186656485805</v>
       </c>
-      <c r="S23" s="9">
+      <c r="S23">
         <v>0.12533238629285828</v>
       </c>
-      <c r="T23" s="9">
+      <c r="T23">
         <v>1.5708207053862253E-2</v>
       </c>
     </row>
@@ -3971,21 +4219,12 @@
       <c r="G24" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
       <c r="L24" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
       <c r="Q24" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -4006,21 +4245,12 @@
       <c r="G25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
       <c r="L25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
       <c r="Q25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -4041,37 +4271,37 @@
       <c r="G26" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26">
         <v>2.9393876913398138</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26">
         <v>8.64</v>
       </c>
       <c r="L26" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="9">
-        <v>4</v>
-      </c>
-      <c r="N26" s="9">
+      <c r="M26">
+        <v>4</v>
+      </c>
+      <c r="N26">
         <v>0</v>
       </c>
-      <c r="O26" s="9">
+      <c r="O26">
         <v>0</v>
       </c>
       <c r="Q26" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R26" s="9">
+      <c r="R26">
         <v>18.399999999999999</v>
       </c>
-      <c r="S26" s="9">
+      <c r="S26">
         <v>2.7276363393971712</v>
       </c>
-      <c r="T26" s="9">
+      <c r="T26">
         <v>7.44</v>
       </c>
     </row>
@@ -4094,21 +4324,12 @@
       <c r="G27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
       <c r="L27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
       <c r="Q27" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -4129,37 +4350,37 @@
       <c r="G28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28">
         <v>1</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28">
         <v>0</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28">
         <v>0</v>
       </c>
       <c r="L28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M28" s="9">
+      <c r="M28">
         <v>4.5999999999999996</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N28">
         <v>0.4898979485566356</v>
       </c>
-      <c r="O28" s="9">
+      <c r="O28">
         <v>0.24</v>
       </c>
       <c r="Q28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R28" s="9">
+      <c r="R28">
         <v>19.399999999999999</v>
       </c>
-      <c r="S28" s="9">
+      <c r="S28">
         <v>2.5768197453450252</v>
       </c>
-      <c r="T28" s="9">
+      <c r="T28">
         <v>6.64</v>
       </c>
     </row>
@@ -4182,21 +4403,12 @@
       <c r="G29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
       <c r="L29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
       <c r="Q29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -4217,37 +4429,37 @@
       <c r="G30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="9">
-        <v>4</v>
-      </c>
-      <c r="I30" s="9">
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
         <v>2.5298221281347035</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30">
         <v>6.4</v>
       </c>
       <c r="L30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M30" s="9">
+      <c r="M30">
         <v>4.2</v>
       </c>
-      <c r="N30" s="9">
+      <c r="N30">
         <v>0.4</v>
       </c>
-      <c r="O30" s="9">
+      <c r="O30">
         <v>0.16</v>
       </c>
       <c r="Q30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="R30" s="9">
+      <c r="R30">
         <v>17</v>
       </c>
-      <c r="S30" s="9">
+      <c r="S30">
         <v>0.89442719099991586</v>
       </c>
-      <c r="T30" s="9">
+      <c r="T30">
         <v>0.8</v>
       </c>
     </row>
@@ -4354,9 +4566,6 @@
       <c r="G35" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -4377,9 +4586,6 @@
       <c r="G36" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -4400,13 +4606,13 @@
       <c r="G37" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37">
         <v>44.2</v>
       </c>
-      <c r="I37" s="9">
+      <c r="I37">
         <v>9.3252345814998137</v>
       </c>
-      <c r="J37" s="9">
+      <c r="J37">
         <v>86.96</v>
       </c>
     </row>
@@ -4429,9 +4635,6 @@
       <c r="G38" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -4452,13 +4655,13 @@
       <c r="G39" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39">
         <v>49.2</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39">
         <v>10.495713410721541</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39">
         <v>110.16</v>
       </c>
     </row>
@@ -4481,9 +4684,6 @@
       <c r="G40" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -4504,13 +4704,13 @@
       <c r="G41" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41">
         <v>36.799999999999997</v>
       </c>
-      <c r="I41" s="9">
+      <c r="I41">
         <v>19.953946977979069</v>
       </c>
-      <c r="J41" s="9">
+      <c r="J41">
         <v>398.16</v>
       </c>
     </row>
@@ -4533,9 +4733,6 @@
       <c r="G42" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -4556,9 +4753,6 @@
       <c r="G43" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
@@ -4579,13 +4773,13 @@
       <c r="G44" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44">
         <v>0.24019746782676341</v>
       </c>
-      <c r="I44" s="9">
+      <c r="I44">
         <v>0.10671333470125648</v>
       </c>
-      <c r="J44" s="9">
+      <c r="J44">
         <v>1.138773580306239E-2</v>
       </c>
     </row>
@@ -4608,13 +4802,13 @@
       <c r="G45" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45">
         <v>0.30492784180589017</v>
       </c>
-      <c r="I45" s="9">
+      <c r="I45">
         <v>0.10947624940423326</v>
       </c>
-      <c r="J45" s="9">
+      <c r="J45">
         <v>1.1985049183617882E-2</v>
       </c>
     </row>
@@ -4637,9 +4831,6 @@
       <c r="G46" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
@@ -4660,13 +4851,13 @@
       <c r="G47" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47">
         <v>0.24670277002517799</v>
       </c>
-      <c r="I47" s="9">
+      <c r="I47">
         <v>2.9572619533334222E-2</v>
       </c>
-      <c r="J47" s="9">
+      <c r="J47">
         <v>8.745398260633408E-4</v>
       </c>
     </row>
@@ -4689,13 +4880,13 @@
       <c r="G48" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H48" s="9">
+      <c r="H48">
         <v>0.27519882405469404</v>
       </c>
-      <c r="I48" s="9">
+      <c r="I48">
         <v>5.6784868686894752E-2</v>
       </c>
-      <c r="J48" s="9">
+      <c r="J48">
         <v>3.22452131178788E-3</v>
       </c>
     </row>
@@ -4718,9 +4909,6 @@
       <c r="G49" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
@@ -4741,13 +4929,13 @@
       <c r="G50" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H50" s="9">
+      <c r="H50">
         <v>0.33281364890198695</v>
       </c>
-      <c r="I50" s="9">
+      <c r="I50">
         <v>8.1574742370374126E-2</v>
       </c>
-      <c r="J50" s="9">
+      <c r="J50">
         <v>6.6544385927929106E-3</v>
       </c>
     </row>
@@ -4770,13 +4958,13 @@
       <c r="G51" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H51">
         <v>0.37342538627981758</v>
       </c>
-      <c r="I51" s="9">
+      <c r="I51">
         <v>0.10454453872141763</v>
       </c>
-      <c r="J51" s="9">
+      <c r="J51">
         <v>1.092956057647399E-2</v>
       </c>
     </row>
@@ -4799,9 +4987,6 @@
       <c r="G52" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
@@ -4822,9 +5007,6 @@
       <c r="G53" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
-      <c r="J53" s="9"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
@@ -4845,13 +5027,13 @@
       <c r="G54" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H54" s="9">
+      <c r="H54">
         <v>44.8</v>
       </c>
-      <c r="I54" s="9">
+      <c r="I54">
         <v>3.6551333764994132</v>
       </c>
-      <c r="J54" s="9">
+      <c r="J54">
         <v>13.36</v>
       </c>
     </row>
@@ -4874,9 +5056,6 @@
       <c r="G55" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
-      <c r="J55" s="9"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
@@ -4897,13 +5076,13 @@
       <c r="G56" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H56" s="9">
+      <c r="H56">
         <v>44</v>
       </c>
-      <c r="I56" s="9">
+      <c r="I56">
         <v>3.2249030993194201</v>
       </c>
-      <c r="J56" s="9">
+      <c r="J56">
         <v>10.4</v>
       </c>
     </row>
@@ -4926,9 +5105,6 @@
       <c r="G57" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
@@ -4949,13 +5125,13 @@
       <c r="G58" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H58" s="9">
+      <c r="H58">
         <v>44.2</v>
       </c>
-      <c r="I58" s="9">
+      <c r="I58">
         <v>4.7074409183759283</v>
       </c>
-      <c r="J58" s="9">
+      <c r="J58">
         <v>22.16</v>
       </c>
     </row>
@@ -8172,4 +8348,453 @@
     <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC204079-5A8D-9F4A-8109-1B56BCEE7401}">
+  <dimension ref="B2:N46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="6" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I8" s="8"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="8"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="8"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="17"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I15" s="17"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I16" s="8"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="16"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B21" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I24" s="17"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I25" s="8"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I27" s="16"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I30" s="17"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I31" s="8"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I32" s="8"/>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I33" s="17"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+    </row>
+    <row r="34" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I35" s="8"/>
+    </row>
+    <row r="38" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I38" s="17"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+    </row>
+    <row r="39" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I41" s="17"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+    </row>
+    <row r="42" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I44" s="17"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16"/>
+    </row>
+    <row r="45" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="9:12" x14ac:dyDescent="0.2">
+      <c r="I46" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:H18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>